<commit_message>
Fix 107 and 89
</commit_message>
<xml_diff>
--- a/P0089/09_FICHAS/N3-FD-General.xlsx
+++ b/P0089/09_FICHAS/N3-FD-General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28619"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejaverianaedu-my.sharepoint.com/personal/crivera_javeriana_edu_co/Documents/Mojana control de archivos/REV_FICHAS/FICHAS/P0089/09_FICHAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="13_ncr:1_{86A57316-0C69-4C5F-8347-1C68770976BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42A376C2-C9F0-4F04-9A91-7C1BAE35200A}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{86A57316-0C69-4C5F-8347-1C68770976BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3347AFF4-F30E-4D1C-8DA3-88608D47997B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
     <t>Anexo 13. Mapa de localización del proyecto.</t>
   </si>
   <si>
-    <t>s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0089/02_PRODUCTOS/3. Documento técnico soporte del proyecto\Anexo 13. Mapa de localización del proyecto..pdf</t>
+    <t>s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0089/02_PRODUCTOS/3. Documento técnico soporte del proyecto/Anexo 13. Mapa de localización del proyecto..pdf</t>
   </si>
   <si>
     <t>El archivo pdf presenta el mapa de la localización del proyecto en términos muy generales, en donde se abarca toda la región de la Mojana</t>
@@ -437,17 +437,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +732,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -744,758 +745,763 @@
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="102.7109375" customWidth="1"/>
+    <col min="16" max="16" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" ht="15">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" ht="15">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>2023</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="2"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:18" ht="15">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>9999</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="N3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:18" ht="15">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>9999</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>9999</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="K5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="9" customFormat="1" ht="15">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:18" s="3" customFormat="1" ht="15">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="9">
         <v>9999</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="K6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:18" ht="15">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="6">
         <v>9999</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="K7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="4" t="s">
+      <c r="N7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:18" ht="15">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <v>9999</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="K8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="4" t="s">
+      <c r="N8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:18" ht="15">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="5">
         <v>9999</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="K9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9" s="4" t="s">
+      <c r="N9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:18" ht="15">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="5">
         <v>9999</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="K10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="4" t="s">
+      <c r="N10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:18" ht="15">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <v>9999</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="K11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O11" s="4" t="s">
+      <c r="N11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:18" ht="15">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="5">
         <v>9999</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="2" t="s">
+      <c r="K12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" s="4" t="s">
+      <c r="N12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:18" ht="15">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="5">
         <v>9999</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" s="4" t="s">
+      <c r="K13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="P13" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="9" customFormat="1" ht="15">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:18" s="3" customFormat="1" ht="15">
+      <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="8">
         <v>9999</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" s="8" t="s">
+      <c r="K14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:18" ht="15">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="5">
         <v>9999</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="4" t="s">
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O15" s="4" t="s">
+      <c r="K15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="7" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ficha N1, n2 y n3 completas
</commit_message>
<xml_diff>
--- a/P0089/09_FICHAS/N3-FD-General.xlsx
+++ b/P0089/09_FICHAS/N3-FD-General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejaverianaedu-my.sharepoint.com/personal/crivera_javeriana_edu_co/Documents/Mojana control de archivos/REV_FICHAS/FICHAS/P0089/09_FICHAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{86A57316-0C69-4C5F-8347-1C68770976BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3347AFF4-F30E-4D1C-8DA3-88608D47997B}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="13_ncr:1_{86A57316-0C69-4C5F-8347-1C68770976BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C8F6CF5-1D72-47E2-8087-0F7D7EA5777F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,18 +437,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +731,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -740,7 +739,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
@@ -804,704 +803,704 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="1">
         <v>2023</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="7" t="s">
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="1">
         <v>9999</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="7" t="s">
+      <c r="N3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="1">
         <v>9999</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="7" t="s">
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="1">
         <v>9999</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="6" t="s">
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="7" t="s">
+      <c r="N5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="3" customFormat="1" ht="15">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>9999</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="10" t="s">
+      <c r="K6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>9999</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="6" t="s">
+      <c r="K7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="7" t="s">
+      <c r="N7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="1">
         <v>9999</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="6" t="s">
+      <c r="K8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="7" t="s">
+      <c r="N8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="1">
         <v>9999</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="K9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9" s="7" t="s">
+      <c r="N9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="1">
         <v>9999</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="7" t="s">
+      <c r="N10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="1">
         <v>9999</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O11" s="7" t="s">
+      <c r="N11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="1">
         <v>9999</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" s="7" t="s">
+      <c r="N12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="P12" s="7" t="s">
+      <c r="P12" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="1">
         <v>9999</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" s="7" t="s">
+      <c r="K13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="P13" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>9999</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" s="10" t="s">
+      <c r="K14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="1">
         <v>9999</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O15" s="7" t="s">
+      <c r="K15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P15" s="6" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>